<commit_message>
Atualizei as medidas das dependências do CAIC calculadas segundo a planta baixa.
</commit_message>
<xml_diff>
--- a/Planta baixa do CAIC/Descrição das salas do CAIC.xlsx
+++ b/Planta baixa do CAIC/Descrição das salas do CAIC.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OtaciliodeAraújo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OtaciliodeAraújo\Documents\workspace\tsi-ppc\Planta baixa do CAIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340"/>
   </bookViews>
   <sheets>
     <sheet name="Prancha 03 06" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="71">
   <si>
     <t>Oficina de artes plásticas</t>
   </si>
@@ -221,6 +221,24 @@
   </si>
   <si>
     <t>Uso atual</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Coordenação de curso</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Total Geral</t>
+  </si>
+  <si>
+    <t>banheiros (11)</t>
+  </si>
+  <si>
+    <t>1,85 x 2,50</t>
   </si>
 </sst>
 </file>
@@ -244,12 +262,42 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -264,7 +312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -272,10 +320,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,10 +626,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,7 +639,7 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -580,152 +650,225 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
+      <c r="B6" s="7" t="s">
+        <v>46</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
+      <c r="B7" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="E10">
+        <f>25*6.24</f>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>5*4.42</f>
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="8"/>
+      <c r="C13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13">
+        <f>5*4.42</f>
+        <v>22.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
+      <c r="B14" s="8"/>
       <c r="C14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D14">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16">
+        <f>SUM(D5:D15)</f>
+        <v>169.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17">
+        <f>1.85*2.5</f>
+        <v>4.625</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="D6" formula="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +878,7 @@
     <col min="3" max="3" width="11" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -746,141 +889,212 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="7" t="s">
         <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>46</v>
       </c>
+      <c r="B5" s="7"/>
       <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="D5">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="G6">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="G7">
+        <f>10*6.25</f>
+        <v>62.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="B8" s="7"/>
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="D8">
+        <f>5*6.25</f>
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="F9">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="12" t="s">
         <v>54</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="F10">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="E11">
+        <f>15*6.25</f>
+        <v>93.75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="E12">
+        <f>12.5*6.25</f>
+        <v>78.125</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="7" t="s">
         <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="D13">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="D14">
+        <f>2.5*6.25</f>
+        <v>15.625</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15">
+        <f>SUM(D2:D14)</f>
+        <v>156.25</v>
+      </c>
+      <c r="E15">
+        <f>SUM(E11:E12)</f>
+        <v>171.875</v>
+      </c>
+      <c r="F15">
+        <f>SUM(F9:F10)+'Prancha 03 06'!D17*2</f>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -890,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,9 +1115,10 @@
     <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -914,147 +1129,179 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="4" t="s">
         <v>38</v>
       </c>
       <c r="C8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+      <c r="H10">
+        <f>'Prancha 04 06'!G6+'Prancha 04 06'!G7+'Prancha 05 06'!G10</f>
+        <v>156.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="9" t="s">
         <v>39</v>
       </c>
       <c r="C11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <f>7.5*6.25</f>
+        <v>46.875</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C13" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15">
+        <f>SUM(D2:D14)</f>
+        <v>93.75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15">
+        <f>'Prancha 03 06'!D16+'Prancha 04 06'!D15+'Prancha 05 06'!D15</f>
+        <v>419.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>